<commit_message>
updated comparison sheet with comments
</commit_message>
<xml_diff>
--- a/OWID/cum_cases_vs_full_vax_percentage_from_OWID.xlsx
+++ b/OWID/cum_cases_vs_full_vax_percentage_from_OWID.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\OWID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A6C32B-7B6F-4320-AB60-8EBEFB5202C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9D1760-5FE2-4885-B6FA-29C35ABBAF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2DD49E5C-6E46-4A69-AC5C-A13F282DAB20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2DD49E5C-6E46-4A69-AC5C-A13F282DAB20}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
     <sheet name="vaccination rate" sheetId="2" r:id="rId2"/>
-    <sheet name="Merge1" sheetId="6" r:id="rId3"/>
-    <sheet name="NOtes" sheetId="7" r:id="rId4"/>
+    <sheet name="merge" sheetId="6" r:id="rId3"/>
+    <sheet name="Notes" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cases'!$A$1:$D$251</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'vaccination rate'!$A$1:$D$1</definedName>
-    <definedName name="ExternalData_2" localSheetId="2" hidden="1">Merge1!$A$1:$C$225</definedName>
+    <definedName name="ExternalData_2" localSheetId="2" hidden="1">merge!$A$1:$C$225</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -2204,7 +2204,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Merge1!$C$1</c:f>
+              <c:f>merge!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2237,7 +2237,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Merge1!$B$2:$B$225</c:f>
+              <c:f>merge!$B$2:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="224"/>
@@ -2918,7 +2918,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Merge1!$C$2:$C$225</c:f>
+              <c:f>merge!$C$2:$C$225</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="224"/>
@@ -11478,8 +11478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E92CF5-C63F-4CF5-BF01-27000CFFAE3B}">
   <dimension ref="A1:C225"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="R89" sqref="R89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C34:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13977,7 +13977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA57515-C211-420B-B1EC-E5C20012BF34}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>